<commit_message>
fixed bug in CSR data file load, removed time from measurement date field (it can be specified in either start time or in data file)
</commit_message>
<xml_diff>
--- a/curator_data/examples/T3/CSRinT3_Sp1_Annotation.xlsx
+++ b/curator_data/examples/T3/CSRinT3_Sp1_Annotation.xlsx
@@ -1,17 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4505"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20910"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="18620" yWindow="2720" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
+    <workbookView xWindow="560" yWindow="560" windowWidth="25040" windowHeight="15500" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="130407" concurrentCalc="0"/>
   <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
   </extLst>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="29">
   <si>
     <t>Parameter</t>
   </si>
@@ -79,9 +79,6 @@
     <t>Spectrometer System</t>
   </si>
   <si>
-    <t>UCD_WUEoptimzed_Channel1</t>
-  </si>
-  <si>
     <t>This entry is defined in the "System Name" of the "CSR Spectrometer System"</t>
   </si>
   <si>
@@ -91,10 +88,22 @@
     <t>CAP-2_2012_Aberdeen</t>
   </si>
   <si>
-    <t>5/7/2012 15:00</t>
-  </si>
-  <si>
     <t>24hr format. This will be ignored if the time is included in the raw data file</t>
+  </si>
+  <si>
+    <t>use PO number from www.plantontology.org</t>
+  </si>
+  <si>
+    <t>Measurement date time</t>
+  </si>
+  <si>
+    <t>UCD_WUEoptimized_Channel1</t>
+  </si>
+  <si>
+    <t>5/7/2012</t>
+  </si>
+  <si>
+    <t>PO:0007016</t>
   </si>
   <si>
     <r>
@@ -116,29 +125,18 @@
         <rFont val="Calibri"/>
         <family val="2"/>
       </rPr>
-      <t xml:space="preserve"> with no leading zeros, e.g. "5/7/2012". The time is in 24hr format</t>
+      <t xml:space="preserve"> with no leading zeros, e.g. "5/7/2012".</t>
     </r>
-  </si>
-  <si>
-    <t>use PO number from www.plantontology.org</t>
-  </si>
-  <si>
-    <t>Measurement date time</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="6">
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="41" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="1">
     <numFmt numFmtId="164" formatCode="h:mm;@"/>
-    <numFmt numFmtId="165" formatCode="0000000"/>
   </numFmts>
-  <fonts count="9">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -231,7 +229,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -244,9 +242,6 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -259,7 +254,13 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -269,7 +270,7 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium9"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
 </styleSheet>
 </file>
 
@@ -594,14 +595,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13:XFD13"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="50.5" customWidth="1"/>
     <col min="2" max="2" width="32.6640625" style="4" customWidth="1"/>
@@ -613,7 +614,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="3"/>
-      <c r="D1" s="11" t="s">
+      <c r="D1" s="10" t="s">
         <v>14</v>
       </c>
     </row>
@@ -622,10 +623,10 @@
         <v>1</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -638,53 +639,53 @@
     </row>
     <row r="4" spans="1:4">
       <c r="A4" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="B4" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="D4" s="9" t="s">
-        <v>25</v>
+        <v>24</v>
+      </c>
+      <c r="B4" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="D4" s="8" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="5" spans="1:4">
       <c r="A5" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="12">
-        <v>7016</v>
+      <c r="B5" s="13" t="s">
+        <v>27</v>
       </c>
       <c r="D5" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
     </row>
     <row r="6" spans="1:4">
       <c r="A6" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B6" s="6">
+      <c r="B6" s="11">
         <v>0.54236111111111118</v>
       </c>
       <c r="D6" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="7" spans="1:4">
       <c r="A7" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="B7" s="6">
+      <c r="B7" s="11">
         <v>0.58402777777777781</v>
       </c>
       <c r="D7" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="8" spans="1:4">
       <c r="A8" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B8" s="5">
+      <c r="B8" s="12">
         <v>10</v>
       </c>
       <c r="D8" t="s">
@@ -704,10 +705,10 @@
         <v>18</v>
       </c>
       <c r="B10" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="D10" s="7" t="s">
         <v>19</v>
-      </c>
-      <c r="D10" s="8" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="11" spans="1:4">
@@ -730,7 +731,7 @@
       <c r="A13" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B13" s="7" t="s">
+      <c r="B13" s="6" t="s">
         <v>12</v>
       </c>
     </row>
@@ -743,11 +744,10 @@
       </c>
     </row>
   </sheetData>
-  <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
     </ext>
   </extLst>

</xml_diff>

<commit_message>
fixed bug in CSR data file load, removed time from measurement date field (it can be specified in either start time or in data file), added growth stage name
</commit_message>
<xml_diff>
--- a/curator_data/examples/T3/CSRinT3_Sp1_Annotation.xlsx
+++ b/curator_data/examples/T3/CSRinT3_Sp1_Annotation.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="32">
   <si>
     <t>Parameter</t>
   </si>
@@ -127,6 +127,15 @@
       </rPr>
       <t xml:space="preserve"> with no leading zeros, e.g. "5/7/2012".</t>
     </r>
+  </si>
+  <si>
+    <t>Growth Stage name</t>
+  </si>
+  <si>
+    <t>whole plant flowering stage</t>
+  </si>
+  <si>
+    <t>use PO name from www.plantontology.org</t>
   </si>
 </sst>
 </file>
@@ -596,10 +605,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D14"/>
+  <dimension ref="A1:D15"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -661,21 +670,21 @@
     </row>
     <row r="6" spans="1:4">
       <c r="A6" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="B6" s="11">
-        <v>0.54236111111111118</v>
+        <v>29</v>
+      </c>
+      <c r="B6" s="13" t="s">
+        <v>30</v>
       </c>
       <c r="D6" t="s">
-        <v>22</v>
+        <v>31</v>
       </c>
     </row>
     <row r="7" spans="1:4">
       <c r="A7" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B7" s="11">
-        <v>0.58402777777777781</v>
+        <v>0.54236111111111118</v>
       </c>
       <c r="D7" t="s">
         <v>22</v>
@@ -683,63 +692,74 @@
     </row>
     <row r="8" spans="1:4">
       <c r="A8" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B8" s="12">
-        <v>10</v>
+        <v>17</v>
+      </c>
+      <c r="B8" s="11">
+        <v>0.58402777777777781</v>
       </c>
       <c r="D8" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
     </row>
     <row r="9" spans="1:4">
       <c r="A9" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B9" s="5" t="s">
-        <v>11</v>
+        <v>10</v>
+      </c>
+      <c r="B9" s="12">
+        <v>10</v>
+      </c>
+      <c r="D9" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="10" spans="1:4">
       <c r="A10" s="2" t="s">
-        <v>18</v>
+        <v>4</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="D10" s="7" t="s">
-        <v>19</v>
+        <v>11</v>
       </c>
     </row>
     <row r="11" spans="1:4">
       <c r="A11" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B11" s="5">
-        <v>5</v>
+        <v>18</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="D11" s="7" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="12" spans="1:4">
       <c r="A12" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B12" s="5">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="13" spans="1:4">
       <c r="A13" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B13" s="6" t="s">
-        <v>12</v>
+        <v>6</v>
+      </c>
+      <c r="B13" s="5">
+        <v>10</v>
       </c>
     </row>
     <row r="14" spans="1:4">
       <c r="A14" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B14" s="6" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4">
+      <c r="A15" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B14" s="4" t="s">
+      <c r="B15" s="4" t="s">
         <v>13</v>
       </c>
     </row>

</xml_diff>